<commit_message>
VBScript class is in development
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr codeName="ЦяКнига" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\simplekitchen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FEE2829-A7C9-415E-9037-C1C8DC63F6B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{533801B8-1794-4268-9FF1-81C1495FF83A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{FDFF3591-85E3-4823-83E1-545037BEC008}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5220" xr2:uid="{96B94350-A670-4A50-A0DA-2787C92C562E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +66,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -76,9 +82,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Офіс">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -116,7 +122,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Офіс">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -222,7 +228,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Офіс">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -371,8 +377,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8613F3BF-820D-4E36-AA53-F7A759C08427}">
-  <sheetPr codeName="Аркуш1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF134D79-D07F-4949-AF64-7C4E98AA325F}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
sheetBuilderStart is renamed into SBStart; new SBReference class in development
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr codeName="ЦяКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\simplekitchen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{533801B8-1794-4268-9FF1-81C1495FF83A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5CDFF0A-193A-4FA2-9278-B83B790B01F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5220" xr2:uid="{96B94350-A670-4A50-A0DA-2787C92C562E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" xr2:uid="{A8B19910-9065-4226-AA33-3FD29E9880FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -66,7 +60,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -82,9 +76,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Офіс">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -122,7 +116,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Офіс">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -228,7 +222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Офіс">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -377,8 +371,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF134D79-D07F-4949-AF64-7C4E98AA325F}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49D864D-C082-4BC9-AAF3-23C000716E53}">
+  <sheetPr codeName="Аркуш1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>